<commit_message>
change manager property manually
</commit_message>
<xml_diff>
--- a/Tests/Validation/SPRUM/ObsAllData.xlsx
+++ b/Tests/Validation/SPRUM/ObsAllData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\GitHubRepos\ApsimX\Tests\Validation\SPRUM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8F4354B-E170-4A48-B6C8-16497C198DE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B8019ED-828C-437C-8161-5DC1CEDB52A4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Observed" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$D$1:$D$1716</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Observed!$I$1:$I$1647</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -510,8 +510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:P1647"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="H1" zoomScale="137" zoomScaleNormal="220" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+    <sheetView tabSelected="1" topLeftCell="A1639" zoomScale="137" zoomScaleNormal="220" workbookViewId="0">
+      <selection activeCell="A1648" sqref="A1648:XFD1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>